<commit_message>
Added logic for getting information from each item and save all the information in Excel Workbook
</commit_message>
<xml_diff>
--- a/resources/files/articles.xlsx
+++ b/resources/files/articles.xlsx
@@ -27,99 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>articles</t>
   </si>
   <si>
     <t xml:space="preserve">Mini portable projector  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motion sensor LED light for closets  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professional makeup brush set  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti-theft backpack with USB charging port  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">French press coffee maker  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retro lava lamp  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunrise alarm clock  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herb growing kit  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ergonomic laptop stand  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neck pillow for travel  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smart thermos bottle with temperature display  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnetic knife block set  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3D wooden puzzle for adults  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED magnifying glass  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB charger hidden spy camera  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wireless charging desk lamp  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cable and charger organizer case  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automatic soap dispenser  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acupressure mat set  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIY candle making kit  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portable solar charger  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Military tactical backpack  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGB LED strip lights with remote  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aromatherapy humidifier diffuser  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collapsible water bottle  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-free reading magnifier glasses  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mini thermal printer for notes  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credit card multi-tool  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waterproof phone pouch  </t>
-  </si>
-  <si>
-    <t>Paint by numbers kit for adults</t>
   </si>
 </sst>
 </file>
@@ -1026,13 +939,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1293,13 +1199,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="48.4285714285714" style="1" customWidth="1"/>
   </cols>
@@ -1314,151 +1220,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>